<commit_message>
V2 Intermediate Excel Skills, Tips and Tricks
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Riki Documents\Coding\Excel Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DDE606F-E9B6-4217-8FF3-E7C2D33544A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8333632-3ED2-429E-832D-BE2D6BB9D156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23940" yWindow="3885" windowWidth="9570" windowHeight="6750" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
+    <workbookView xWindow="19230" yWindow="3885" windowWidth="9570" windowHeight="6750" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$F$26</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>Movie Inventory</t>
   </si>
@@ -154,13 +157,28 @@
   </si>
   <si>
     <t>The Lion, The Witch, and the Wardrobe</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Average:</t>
+  </si>
+  <si>
+    <t>Lowest:</t>
+  </si>
+  <si>
+    <t>Highest:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +204,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,13 +239,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,23 +566,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A1D6D3-1FAE-43D7-9469-467D059B2D84}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -554,7 +593,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -564,7 +603,7 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -574,218 +613,236 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>2011</v>
+        <v>1999</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>2002</v>
+        <v>2009</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
-        <v>3</v>
+      <c r="D6" s="5">
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B7">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B8">
-        <v>2009</v>
+        <v>2002</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2007</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10">
-        <v>2009</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>2015</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D11" s="5">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
         <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>2017</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I11" s="8"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B13">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D13" s="5">
+        <v>9</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -794,58 +851,58 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B14">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14">
-        <v>15</v>
+      <c r="D14" s="5">
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>2000</v>
+        <v>2017</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="D15" s="5">
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B16">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16">
-        <v>4</v>
+      <c r="D16" s="5">
+        <v>5</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -856,19 +913,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="D17" s="5">
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
@@ -876,19 +933,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>1997</v>
+        <v>2016</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
         <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
@@ -896,7 +953,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>1999</v>
@@ -904,11 +961,11 @@
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19">
-        <v>6</v>
+      <c r="D19" s="5">
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -916,19 +973,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B20">
-        <v>2003</v>
+        <v>2011</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D20" s="5">
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
@@ -936,51 +993,102 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="D21">
-        <v>2</v>
+      <c r="D21" s="5">
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22">
-        <v>5</v>
+      <c r="D22" s="5">
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
+      <c r="C23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="7">
+        <f>SUM(D3:D22)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="7">
+        <f>AVERAGE(D3:D22)</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="7">
+        <f>MAX(D3:D22)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="7">
+        <f>MIN(D3:D22)</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:F26" xr:uid="{F1A1D6D3-1FAE-43D7-9469-467D059B2D84}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F26">
+    <sortCondition ref="A3:A26"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="D3:D22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
V3 Advanced Excel - VLOOKUP Basics
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Riki Documents\Coding\Excel Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8333632-3ED2-429E-832D-BE2D6BB9D156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14409CD9-C0C7-42FA-947A-23D827B44D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19230" yWindow="3885" windowWidth="9570" windowHeight="6750" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
+    <workbookView xWindow="14430" yWindow="45" windowWidth="14445" windowHeight="15750" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t>Movie Inventory</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Highest:</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -235,23 +238,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,9 +623,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A1D6D3-1FAE-43D7-9469-467D059B2D84}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,20 +633,21 @@
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -603,7 +659,7 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -623,7 +679,7 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>5</v>
       </c>
       <c r="E3" t="s">
@@ -632,8 +688,8 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -645,7 +701,7 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
@@ -654,8 +710,8 @@
       <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -667,7 +723,7 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>6</v>
       </c>
       <c r="E5" t="s">
@@ -676,10 +732,10 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -689,7 +745,7 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -698,8 +754,8 @@
       <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -711,7 +767,7 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>10</v>
       </c>
       <c r="E7" t="s">
@@ -720,10 +776,15 @@
       <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -733,7 +794,7 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>2</v>
       </c>
       <c r="E8" t="s">
@@ -742,8 +803,14 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
+      <c r="H8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="13" t="str">
+        <f>VLOOKUP(H8,A3:F22,3,FALSE)</f>
+        <v>PG</v>
+      </c>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -755,7 +822,7 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>5</v>
       </c>
       <c r="E9" t="s">
@@ -764,8 +831,8 @@
       <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -777,7 +844,7 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>5</v>
       </c>
       <c r="E10" t="s">
@@ -786,8 +853,8 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -799,7 +866,7 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>4</v>
       </c>
       <c r="E11" t="s">
@@ -808,8 +875,8 @@
       <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -821,7 +888,7 @@
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>15</v>
       </c>
       <c r="E12" t="s">
@@ -841,7 +908,7 @@
       <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>9</v>
       </c>
       <c r="E13" t="s">
@@ -861,7 +928,7 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>2</v>
       </c>
       <c r="E14" t="s">
@@ -881,7 +948,7 @@
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>14</v>
       </c>
       <c r="E15" t="s">
@@ -901,7 +968,7 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>5</v>
       </c>
       <c r="E16" t="s">
@@ -921,7 +988,7 @@
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>9</v>
       </c>
       <c r="E17" t="s">
@@ -941,7 +1008,7 @@
       <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>6</v>
       </c>
       <c r="E18" t="s">
@@ -961,7 +1028,7 @@
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>7</v>
       </c>
       <c r="E19" t="s">
@@ -981,7 +1048,7 @@
       <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>6</v>
       </c>
       <c r="E20" t="s">
@@ -1001,7 +1068,7 @@
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>5</v>
       </c>
       <c r="E21" t="s">
@@ -1021,7 +1088,7 @@
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>15</v>
       </c>
       <c r="E22" t="s">
@@ -1033,43 +1100,42 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <f>SUM(D3:D22)</f>
         <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <f>AVERAGE(D3:D22)</f>
         <v>6.75</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <f>MAX(D3:D22)</f>
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <f>MIN(D3:D22)</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F26" xr:uid="{F1A1D6D3-1FAE-43D7-9469-467D059B2D84}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F26">
     <sortCondition ref="A3:A26"/>
   </sortState>

</xml_diff>

<commit_message>
V6 Advanced Excel - Protecting a Sheet
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Riki Documents\Coding\Excel Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14409CD9-C0C7-42FA-947A-23D827B44D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC9712F-6FB0-49DF-A0F7-200667E59181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14430" yWindow="45" windowWidth="14445" windowHeight="15750" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
+    <workbookView xWindow="14175" yWindow="30" windowWidth="14580" windowHeight="15750" activeTab="1" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
   <si>
     <t>Movie Inventory</t>
   </si>
@@ -172,14 +172,66 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Music Inventory</t>
+  </si>
+  <si>
+    <t>Star Rating</t>
+  </si>
+  <si>
+    <t>Blume - Rise From Grey</t>
+  </si>
+  <si>
+    <t>Synthpop</t>
+  </si>
+  <si>
+    <t>The Stabilizeers - Tyranny</t>
+  </si>
+  <si>
+    <t>New Wave</t>
+  </si>
+  <si>
+    <t>Code 64 - Storm</t>
+  </si>
+  <si>
+    <t>Code 64 - Departure</t>
+  </si>
+  <si>
+    <t>B! Machine - Aftermath</t>
+  </si>
+  <si>
+    <t>B! Machine - Hybrid</t>
+  </si>
+  <si>
+    <t>Midnight Resistance - Remote</t>
+  </si>
+  <si>
+    <t>Depeche Mode - Violator</t>
+  </si>
+  <si>
+    <t>Classic Synthpop</t>
+  </si>
+  <si>
+    <t>Alphaville - Forever Young</t>
+  </si>
+  <si>
+    <t>Alphaville - Catching Rays on Giant</t>
+  </si>
+  <si>
+    <t>Cosmicity - Escape Pod for Two</t>
+  </si>
+  <si>
+    <t>Total Value of CDs:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -286,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -296,9 +348,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -307,6 +356,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A1D6D3-1FAE-43D7-9469-467D059B2D84}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -640,14 +701,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -776,10 +837,10 @@
       <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="8"/>
@@ -803,10 +864,10 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="13" t="str">
+      <c r="I8" s="12" t="str">
         <f>VLOOKUP(H8,A3:F22,3,FALSE)</f>
         <v>PG</v>
       </c>
@@ -1162,12 +1223,322 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1BE278-49B5-47CD-BD66-0692418FEB6A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="17">
+        <f>SUM(D3:D13)</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>2007</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="18">
+        <v>155</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>1999</v>
+      </c>
+      <c r="C4">
+        <v>4.5</v>
+      </c>
+      <c r="D4" s="18">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>2011</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="18">
+        <v>300</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>2007</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>2007</v>
+      </c>
+      <c r="C7">
+        <v>4.5</v>
+      </c>
+      <c r="D7" s="18">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>2007</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" s="18">
+        <v>89</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>2012</v>
+      </c>
+      <c r="C9">
+        <v>4.5</v>
+      </c>
+      <c r="D9" s="18">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>1996</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="18">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>1995</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" s="18">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>2014</v>
+      </c>
+      <c r="C12">
+        <v>4.5</v>
+      </c>
+      <c r="D12" s="18">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>2007</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="18">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="18"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V7 Advanced Excel - 3D Formulas
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Riki Documents\Coding\Excel Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC9712F-6FB0-49DF-A0F7-200667E59181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB8ACB3-B01C-4E2F-BA66-C6162FA47FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14175" yWindow="30" windowWidth="14580" windowHeight="15750" activeTab="1" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
+    <workbookView xWindow="14265" yWindow="135" windowWidth="14580" windowHeight="15750" activeTab="1" xr2:uid="{7F9C9991-2303-4BA6-BA0A-8C8BF97D246F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$F$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sheet1 (2)'!$A$2:$F$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="64">
   <si>
     <t>Movie Inventory</t>
   </si>
@@ -223,17 +226,24 @@
   </si>
   <si>
     <t>Total Value of CDs:</t>
+  </si>
+  <si>
+    <t>Total Value of DVDs:</t>
+  </si>
+  <si>
+    <t>Grand Total Value:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +279,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -335,10 +352,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -356,20 +374,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -686,7 +713,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,14 +728,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1222,11 +1249,518 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D404D237-A2C2-4D70-B888-DE1EC9DFC7FE}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="13">
+        <f>SUM(D3:D2000)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>2003</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="14">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="22">
+        <f>SUM('Sheet1 (2):Sheet2'!I2)</f>
+        <v>881</v>
+      </c>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>1999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="14">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2009</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="14">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>2002</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="14">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>2016</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="14">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2007</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="14">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>2015</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="14">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>2017</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="14">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>2010</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="14">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <v>2016</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>2017</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="14">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>2009</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="14">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>1997</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="14">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>2016</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="14">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="14">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20">
+        <v>2011</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="14">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>2015</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="14">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>2008</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="14">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+      <c r="D26" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1BE278-49B5-47CD-BD66-0692418FEB6A}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,21 +1768,21 @@
     <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1260,7 +1794,7 @@
       <c r="C2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1272,9 +1806,9 @@
       <c r="H2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="15">
         <f>SUM(D3:D13)</f>
-        <v>768</v>
+        <v>746</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1287,8 +1821,8 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="18">
-        <v>155</v>
+      <c r="D3" s="16">
+        <v>135</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -1307,7 +1841,7 @@
       <c r="C4">
         <v>4.5</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>49</v>
       </c>
       <c r="E4" t="s">
@@ -1327,7 +1861,7 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>300</v>
       </c>
       <c r="E5" t="s">
@@ -1347,7 +1881,7 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>88</v>
       </c>
       <c r="E6" t="s">
@@ -1367,7 +1901,7 @@
       <c r="C7">
         <v>4.5</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>45</v>
       </c>
       <c r="E7" t="s">
@@ -1387,8 +1921,8 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="18">
-        <v>89</v>
+      <c r="D8" s="16">
+        <v>88</v>
       </c>
       <c r="E8" t="s">
         <v>48</v>
@@ -1407,7 +1941,7 @@
       <c r="C9">
         <v>4.5</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>14</v>
       </c>
       <c r="E9" t="s">
@@ -1427,8 +1961,8 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="18">
-        <v>6</v>
+      <c r="D10" s="16">
+        <v>5</v>
       </c>
       <c r="E10" t="s">
         <v>57</v>
@@ -1447,7 +1981,7 @@
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>5</v>
       </c>
       <c r="E11" t="s">
@@ -1467,7 +2001,7 @@
       <c r="C12">
         <v>4.5</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>12</v>
       </c>
       <c r="E12" t="s">
@@ -1487,7 +2021,7 @@
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>5</v>
       </c>
       <c r="E13" t="s">
@@ -1498,40 +2032,40 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="18"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="18"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="18"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="18"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="18"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="18"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="18"/>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="18"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="18"/>
+      <c r="D22" s="16"/>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="18"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="18"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="18"/>
+      <c r="D25" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -1541,4 +2075,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F6E036-F339-442D-BB3B-C935B69D39BE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>